<commit_message>
Project Restore Tree Excel
</commit_message>
<xml_diff>
--- a/Projects/Restore Tree.xlsx
+++ b/Projects/Restore Tree.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew\Documents\SQL Server Management Studio\Restore Scripts\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B476AF58-2C9E-4B8D-A02A-CBB23428743A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5576E92E-8233-4CC8-9E04-8B86736C7C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Restore Tree" sheetId="1" r:id="rId1"/>
-    <sheet name="Test IDs" sheetId="8" r:id="rId2"/>
-    <sheet name="TableInfo" sheetId="5" r:id="rId3"/>
-    <sheet name="1l diff" sheetId="6" r:id="rId4"/>
-    <sheet name="2l diff" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="Test IDs" sheetId="8" r:id="rId3"/>
+    <sheet name="TableInfo" sheetId="5" r:id="rId4"/>
+    <sheet name="1l diff" sheetId="6" r:id="rId5"/>
+    <sheet name="2l diff" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="238">
   <si>
     <t>LinkObjectToActivityHistory</t>
   </si>
@@ -594,15 +595,9 @@
     <t>78 LinkSkillsToInternalInterview</t>
   </si>
   <si>
-    <t>BEFORE Project List inserts - so triggers don't make new PCS records</t>
-  </si>
-  <si>
     <t>JobRequirements</t>
   </si>
   <si>
-    <t>HANDLED by ah triggers</t>
-  </si>
-  <si>
     <t>LinkOpportunitiesToBusinessObjects</t>
   </si>
   <si>
@@ -633,21 +628,6 @@
     <t>InvoiceItems</t>
   </si>
   <si>
-    <t>from InternalInterviews.TaskID AND Interview.TaskID, not existing</t>
-  </si>
-  <si>
-    <t>DeletedTasks</t>
-  </si>
-  <si>
-    <t>DELETE THESE</t>
-  </si>
-  <si>
-    <t>TaskData</t>
-  </si>
-  <si>
-    <t>not existing - will come in with incorrect Created/Updated On/By (because of Insert trigger)</t>
-  </si>
-  <si>
     <t>RightID</t>
   </si>
   <si>
@@ -657,9 +637,6 @@
     <t>HANDLED (above)</t>
   </si>
   <si>
-    <t>LinkClnInterviewsToResults</t>
-  </si>
-  <si>
     <t>WebJobPostings</t>
   </si>
   <si>
@@ -685,9 +662,6 @@
   </si>
   <si>
     <t>LinkMediaToProject</t>
-  </si>
-  <si>
-    <t>Disable INSERT trigger</t>
   </si>
   <si>
     <t>AFTER Task Restore - set ProjectsID</t>
@@ -704,22 +678,89 @@
   <si>
     <t>Update - reevaluate their proper block after ProjectsCandidateBlocks inserts (many peoples blocks will be set back to this project).
 Report - List of candidates on this project. Block at backup-time, block pre-restore, block post-restore</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>NESTED. from InternalInterviews.TaskID AND Interview.TaskID</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>ListsID</t>
+  </si>
+  <si>
+    <t>Lists</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>SourceTable</t>
+  </si>
+  <si>
+    <t>'Projects')</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>ProjectsID, PeopleID</t>
+  </si>
+  <si>
+    <t>LinkOpportunityToBusObjectID</t>
+  </si>
+  <si>
+    <t>AS CHILD</t>
+  </si>
+  <si>
+    <t>ProjectsID, CompaniesID</t>
+  </si>
+  <si>
+    <t>LinkEventToObjectsID</t>
+  </si>
+  <si>
+    <t>ProjectsID, CompaniesID, PeopleID</t>
+  </si>
+  <si>
+    <t>ProjectsID, PeopleID, WorkListsID</t>
+  </si>
+  <si>
+    <t>handled as child</t>
+  </si>
+  <si>
+    <t>WebPostingsIndustries</t>
+  </si>
+  <si>
+    <t>TaskID = TaskID AND CallCode IS NULL</t>
+  </si>
+  <si>
+    <t>ProjectsID, ProjectStagesID, TaskID</t>
+  </si>
+  <si>
+    <t>LinkIntInterviewsToResultsID</t>
+  </si>
+  <si>
+    <t>WebJobPostingsID, WebSitesID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -866,18 +907,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,11 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1212,7 @@
     <col min="2" max="2" width="33.85546875" style="6" customWidth="1"/>
     <col min="3" max="4" width="31.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="77.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="6" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="93.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.85546875" style="5" customWidth="1"/>
@@ -1235,9 +1276,6 @@
       <c r="B3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
@@ -1257,523 +1295,476 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>186</v>
+        <v>72</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>188</v>
+        <v>63</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>96</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="H17" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="J16" s="6" t="s">
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J17" s="6" t="s">
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="M17" s="5" t="s">
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="6" t="s">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F21" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F22" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E48" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F24" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F25" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="E50" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="6" t="s">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F27" s="6" t="s">
+      <c r="E51" s="5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F28" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="5" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F50" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F51" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F52" s="18"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F53" s="18"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F55" s="18"/>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F56" s="18"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F64" s="18"/>
-    </row>
-    <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="J68" s="4"/>
-    </row>
-    <row r="69" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="J69" s="8"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="J71" s="8"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="18"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="18"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="18"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="18"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="18"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-    </row>
-    <row r="79" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="J79" s="8"/>
-    </row>
-    <row r="80" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="J80" s="10"/>
-    </row>
-    <row r="81" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="J81" s="12"/>
-    </row>
-    <row r="82" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="J82" s="12"/>
-    </row>
-    <row r="83" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="12"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="12"/>
-      <c r="J83" s="12"/>
-    </row>
-    <row r="84" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="12"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="12"/>
-      <c r="J84" s="12"/>
-    </row>
-    <row r="85" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="12"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="12"/>
-      <c r="J85" s="12"/>
-    </row>
-    <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="J86" s="4"/>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+    <row r="53" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="12"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="12"/>
+      <c r="J56" s="12"/>
+    </row>
+    <row r="57" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="12"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="12"/>
+      <c r="J57" s="12"/>
+    </row>
+    <row r="58" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="12"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="12"/>
+      <c r="J58" s="12"/>
+    </row>
+    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B62" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F89" s="10"/>
-      <c r="J89" s="10"/>
-    </row>
-    <row r="90" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="20" t="s">
+      <c r="F62" s="10"/>
+      <c r="J62" s="10"/>
+    </row>
+    <row r="63" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F90" s="12"/>
-      <c r="J90" s="12"/>
-    </row>
-    <row r="91" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="14" t="s">
+      <c r="F63" s="12"/>
+      <c r="J63" s="12"/>
+    </row>
+    <row r="64" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F91" s="12"/>
-      <c r="J91" s="12"/>
-    </row>
-    <row r="92" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="15" t="s">
+      <c r="F64" s="12"/>
+      <c r="J64" s="12"/>
+    </row>
+    <row r="65" spans="2:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F92" s="12"/>
-      <c r="J92" s="12"/>
-    </row>
-    <row r="93" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="16" t="s">
+      <c r="F65" s="12"/>
+      <c r="J65" s="12"/>
+    </row>
+    <row r="66" spans="2:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F93" s="4"/>
-      <c r="J93" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="J66" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1782,6 +1773,522 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BEA3AE-C239-4ABD-9492-6D79F4D5D2D5}">
+  <dimension ref="A1:S41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="str">
+        <f>VLOOKUP(B1,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsCallStatus</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(B2,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectBillingDetails</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(B3,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectInvoices</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="str">
+        <f>VLOOKUP(B4,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsBenchmarkCandidates</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(B5,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsClientEmployeesLists</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(B6,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsClientTeams</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(B7,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsCompaniesLists</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(B8,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsFileSearchCandidates</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="str">
+        <f>VLOOKUP(B9,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsInternalInterviewLists</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP(B10,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsPresentedLists</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="str">
+        <f>VLOOKUP(B11,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsShortLists</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="str">
+        <f>VLOOKUP(B12,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>CandidateReferrals</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="str">
+        <f>VLOOKUP(B13,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsSources</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="str">
+        <f>VLOOKUP(B14,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsTargetLists</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" t="str">
+        <f>VLOOKUP(B15,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsTeam</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="str">
+        <f>VLOOKUP(B16,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>PeopleAppliedTo</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" t="str">
+        <f>VLOOKUP(B17,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LinkMediaToProject</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" t="str">
+        <f>VLOOKUP(B18,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectStages</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" t="str">
+        <f>VLOOKUP(B19,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>JobRequirements</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="str">
+        <f>VLOOKUP(B20,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>InternalInterviews</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" t="str">
+        <f>VLOOKUP(B21,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>WebJobPostings</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" t="str">
+        <f>VLOOKUP(B22,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LinkOpportunitiesToBusinessObjects</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" t="str">
+        <f>VLOOKUP(B23,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LinkEventsToBusinessObjects</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24" t="str">
+        <f>VLOOKUP(B24,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsAccounting</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="str">
+        <f>VLOOKUP(B25,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LastProjectActivity</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="str">
+        <f>VLOOKUP(B26,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectsCandidateBlocks</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="str">
+        <f>VLOOKUP(B27,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>Affiliates</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="str">
+        <f>VLOOKUP(B28,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>CandidateCredentials</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="str">
+        <f>VLOOKUP(B29,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>InternalInterviews</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" t="str">
+        <f>VLOOKUP(B30,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>Interview</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" t="str">
+        <f>VLOOKUP(B31,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ProjectStages</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="e">
+        <f>VLOOKUP(B32,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="str">
+        <f>VLOOKUP(B33,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LinkObjectToActivityHistory</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="str">
+        <f>VLOOKUP(B34,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LinkObjectToDocument</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="str">
+        <f>VLOOKUP(B35,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>LinkObjectToTask</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C36" t="e">
+        <f>VLOOKUP(B36,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="str">
+        <f>VLOOKUP(B37,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>ListsDetails</v>
+      </c>
+      <c r="L37" t="s">
+        <v>218</v>
+      </c>
+      <c r="M37" t="s">
+        <v>219</v>
+      </c>
+      <c r="N37" t="s">
+        <v>216</v>
+      </c>
+      <c r="O37" t="s">
+        <v>220</v>
+      </c>
+      <c r="P37" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>222</v>
+      </c>
+      <c r="R37" t="s">
+        <v>217</v>
+      </c>
+      <c r="S37" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C38" t="e">
+        <f>VLOOKUP(B38,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="str">
+        <f>VLOOKUP(B39,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>People</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="str">
+        <f>VLOOKUP(B40,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>Task</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>213</v>
+      </c>
+      <c r="B41" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" t="str">
+        <f>VLOOKUP(B41,'Restore Tree'!$B$2:$B$57,1, FALSE)</f>
+        <v>WebRequests</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4650E00-41D3-4D18-8520-046A79031E4C}">
   <dimension ref="A1:G79"/>
   <sheetViews>
@@ -3269,12 +3776,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65B7801-4248-4515-8576-2B571CA2AF7A}">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75:I78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,11 +3796,11 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>IF('Restore Tree'!B3&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B3&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Projects'</v>
+        <f>IF('Restore Tree'!B3&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B3&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Projects'</v>
       </c>
       <c r="E1" t="str">
-        <f>IF('Restore Tree'!F3&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F3&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F3&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F3&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I1" t="str">
@@ -3303,11 +3810,11 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>IF('Restore Tree'!B4&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B4&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B4&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B4&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E2" t="str">
-        <f>IF('Restore Tree'!F4&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F4&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F4&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F4&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I2" t="str">
@@ -3317,11 +3824,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>IF('Restore Tree'!B67&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B67&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B5&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B5&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'CandidateCredentials'</v>
       </c>
       <c r="E3" t="str">
-        <f>IF('Restore Tree'!F67&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F67&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F5&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F5&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I3" t="str">
@@ -3330,223 +3837,223 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="e">
+      <c r="A4" t="str">
+        <f>IF('Restore Tree'!B6&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B6&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsCallStatus'</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IF('Restore Tree'!F6&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F6&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <f>IF('Restore Tree'!J7&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J7&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>IF('Restore Tree'!B7&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B7&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'JobRequirements'</v>
+      </c>
+      <c r="E5" t="str">
+        <f>IF('Restore Tree'!F7&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F7&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <f>IF('Restore Tree'!J28&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J28&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>IF('Restore Tree'!B8&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B8&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LastProjectActivity'</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IF('Restore Tree'!F8&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F8&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f>IF('Restore Tree'!J8&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J8&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>IF('Restore Tree'!B9&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B9&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkOpportunitiesToBusinessObjects'</v>
+      </c>
+      <c r="E7" t="str">
+        <f>IF('Restore Tree'!F9&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F9&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I7" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
         <v>#REF!</v>
       </c>
-      <c r="E4" t="e">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>IF('Restore Tree'!B10&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B10&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectBillingDetails'</v>
+      </c>
+      <c r="E8" t="str">
+        <f>IF('Restore Tree'!F10&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F10&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I8" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
         <v>#REF!</v>
       </c>
-      <c r="I4" t="str">
-        <f>IF('Restore Tree'!J6&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J6&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>IF('Restore Tree'!B5&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B5&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'CandidateCredentials'</v>
-      </c>
-      <c r="E5" t="str">
-        <f>IF('Restore Tree'!F5&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F5&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <f>IF('Restore Tree'!J38&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J38&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>IF('Restore Tree'!B25&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B25&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="E6" t="str">
-        <f>IF('Restore Tree'!F25&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F25&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkClnInterviewsToResults'</v>
-      </c>
-      <c r="I6" t="str">
-        <f>IF('Restore Tree'!J7&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J7&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>IF('Restore Tree'!B6&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B6&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'JobRequirements'</v>
-      </c>
-      <c r="E7" t="str">
-        <f>IF('Restore Tree'!F6&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F6&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <f>IF('Restore Tree'!J70&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J70&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>IF('Restore Tree'!B38&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B38&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Affiliates'</v>
-      </c>
-      <c r="E8" t="str">
-        <f>IF('Restore Tree'!F38&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F38&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I8" t="str">
-        <f>IF('Restore Tree'!J39&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J39&amp;"'", "")</f>
-        <v/>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>IF('Restore Tree'!B7&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B7&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LastProjectActivity'</v>
+        <f>IF('Restore Tree'!B11&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B11&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsAccounting'</v>
       </c>
       <c r="E9" t="str">
-        <f>IF('Restore Tree'!F7&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F7&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F11&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F11&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I9" t="str">
-        <f>IF('Restore Tree'!J40&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J40&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J29&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J29&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>IF('Restore Tree'!B70&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B70&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B12&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B12&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsClientTeams'</v>
       </c>
       <c r="E10" t="str">
-        <f>IF('Restore Tree'!F70&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F70&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F12&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F12&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkInterviewersToClientInterview'</v>
       </c>
       <c r="I10" t="str">
-        <f>IF('Restore Tree'!J41&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J41&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J30&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J30&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>IF('Restore Tree'!B39&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B39&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B13&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B13&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsCompaniesLists'</v>
       </c>
       <c r="E11" t="str">
-        <f>IF('Restore Tree'!F39&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F39&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F13&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F13&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectTargetCompaniesCandidates'</v>
       </c>
       <c r="I11" t="str">
-        <f>IF('Restore Tree'!J42&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J42&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J31&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J31&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>IF('Restore Tree'!B40&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B40&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectTargetCompaniesCandidates'</v>
+        <f>IF('Restore Tree'!B14&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B14&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsTeam'</v>
       </c>
       <c r="E12" t="str">
-        <f>IF('Restore Tree'!F40&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F40&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F14&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F14&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I12" t="str">
-        <f>IF('Restore Tree'!J45&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J45&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J34&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J34&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>IF('Restore Tree'!B41&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B41&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsTargetLists'</v>
+        <f>IF('Restore Tree'!B15&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B15&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectStages'</v>
       </c>
       <c r="E13" t="str">
-        <f>IF('Restore Tree'!F41&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F41&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F15&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F15&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkTaskToProjectStages'</v>
       </c>
       <c r="I13" t="str">
-        <f>IF('Restore Tree'!J46&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J46&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J35&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J35&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>IF('Restore Tree'!B42&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B42&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsSources'</v>
+        <f>IF('Restore Tree'!B16&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B16&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectInvoices'</v>
       </c>
       <c r="E14" t="str">
-        <f>IF('Restore Tree'!F42&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F42&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F16&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F16&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'InvoiceItems'</v>
       </c>
       <c r="I14" t="str">
-        <f>IF('Restore Tree'!J47&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J47&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J36&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J36&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>IF('Restore Tree'!B26&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B26&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'WebJobPostings'</v>
+        <f>IF('Restore Tree'!B17&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B17&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'InternalInterviews'</v>
       </c>
       <c r="E15" t="str">
-        <f>IF('Restore Tree'!F26&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F26&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Questions'</v>
+        <f>IF('Restore Tree'!F17&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F17&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Task'</v>
       </c>
       <c r="I15" t="str">
-        <f>IF('Restore Tree'!J48&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J48&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J37&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J37&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f>IF('Restore Tree'!B45&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B45&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsBenchmarkCandidates'</v>
+      <c r="A16" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
       <c r="E16" t="str">
-        <f>IF('Restore Tree'!F45&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F45&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F18&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F18&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkInternalInterviewsToResults'</v>
       </c>
       <c r="I16" t="str">
-        <f>IF('Restore Tree'!J49&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J49&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J38&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J38&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>IF('Restore Tree'!B46&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B46&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'PeopleAppliedTo'</v>
+      <c r="A17" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
       <c r="E17" t="str">
-        <f>IF('Restore Tree'!F46&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F46&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F19&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F19&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkSkillsToInternalInterview'</v>
       </c>
       <c r="I17" t="str">
-        <f>IF('Restore Tree'!J50&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J50&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J39&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J39&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f>IF('Restore Tree'!B47&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B47&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsClientEmployeesLists'</v>
+      <c r="A18" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
       <c r="E18" t="str">
-        <f>IF('Restore Tree'!F47&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F47&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F20&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F20&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Task'</v>
       </c>
       <c r="I18" t="str">
-        <f>IF('Restore Tree'!J51&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J51&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J40&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J40&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f>IF('Restore Tree'!B48&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B48&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsInternalInterviewLists'</v>
+      <c r="A19" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
       <c r="E19" t="str">
-        <f>IF('Restore Tree'!F48&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F48&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'InternalInterviews'</v>
+        <f>IF('Restore Tree'!F21&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F21&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkInterviewersToClientInterview'</v>
       </c>
       <c r="I19" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -3555,697 +4062,697 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>IF('Restore Tree'!B49&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B49&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsShortLists'</v>
+        <f>IF('Restore Tree'!B18&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B18&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E20" t="str">
-        <f>IF('Restore Tree'!F49&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F49&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Interview'</v>
+        <f>IF('Restore Tree'!F22&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F22&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Questions'</v>
       </c>
       <c r="I20" t="str">
-        <f>IF('Restore Tree'!J52&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J52&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J41&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J41&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>IF('Restore Tree'!B50&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B50&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B19&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B19&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E21" t="str">
-        <f>IF('Restore Tree'!F50&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F50&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'CandidateCredentials'</v>
+        <f>IF('Restore Tree'!F23&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F23&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'SkillsQuestions'</v>
       </c>
       <c r="I21" t="str">
-        <f>IF('Restore Tree'!J55&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J55&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J51&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J51&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>IF('Restore Tree'!B51&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B51&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B20&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B20&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Interview'</v>
       </c>
       <c r="E22" t="str">
-        <f>IF('Restore Tree'!F51&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F51&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'CandidateReferences'</v>
-      </c>
-      <c r="I22" t="str">
-        <f>IF('Restore Tree'!J53&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J53&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="e">
+        <f>IF('Restore Tree'!F24&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F24&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkWebPostingToWebSite'</v>
+      </c>
+      <c r="I22" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
         <v>#REF!</v>
       </c>
-      <c r="E23" t="e">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>IF('Restore Tree'!B21&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B21&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <f>IF('Restore Tree'!F25&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F25&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'WebPostingsIndustries'</v>
+      </c>
+      <c r="I23" t="str">
+        <f>IF('Restore Tree'!J9&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J9&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E24" t="str">
+        <f>IF('Restore Tree'!F26&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F26&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I24" t="str">
+        <f>IF('Restore Tree'!J48&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J48&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>IF('Restore Tree'!B22&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B22&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'WebJobPostings'</v>
+      </c>
+      <c r="E25" t="str">
+        <f>IF('Restore Tree'!F27&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F27&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I25" t="str">
+        <f>IF('Restore Tree'!J33&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J33&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>IF('Restore Tree'!B23&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B23&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <f>IF('Restore Tree'!F28&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F28&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <f>IF('Restore Tree'!J32&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J32&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>IF('Restore Tree'!B24&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B24&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f>IF('Restore Tree'!F29&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F29&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I27" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
         <v>#REF!</v>
       </c>
-      <c r="I23" t="str">
-        <f>IF('Restore Tree'!J8&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J8&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>IF('Restore Tree'!B52&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B52&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'CandidateReferrals'</v>
-      </c>
-      <c r="E24" t="str">
-        <f>IF('Restore Tree'!F52&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F52&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I24" t="str">
-        <f>IF('Restore Tree'!J33&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J33&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f>IF('Restore Tree'!B55&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B55&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'WebRequests'</v>
-      </c>
-      <c r="E25" t="str">
-        <f>IF('Restore Tree'!F55&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F55&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I25" t="str">
-        <f>IF('Restore Tree'!J44&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J44&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f>IF('Restore Tree'!B53&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B53&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="E26" t="str">
-        <f>IF('Restore Tree'!F53&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F53&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I26" t="str">
-        <f>IF('Restore Tree'!J43&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J43&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f>IF('Restore Tree'!B8&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B8&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkOpportunitiesToBusinessObjects'</v>
-      </c>
-      <c r="E27" t="str">
-        <f>IF('Restore Tree'!F8&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F8&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I27" t="str">
-        <f>IF('Restore Tree'!J34&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J34&amp;"'", "")</f>
-        <v/>
-      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>IF('Restore Tree'!B33&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B33&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkObjectToDocument'</v>
+        <f>IF('Restore Tree'!B26&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B26&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkEventsToBusinessObjects'</v>
       </c>
       <c r="E28" t="str">
-        <f>IF('Restore Tree'!F33&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F33&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I28" t="str">
-        <f>IF('Restore Tree'!J35&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J35&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F30&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F30&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I28" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>IF('Restore Tree'!B44&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B44&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsPresentedLists'</v>
+        <f>IF('Restore Tree'!B27&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B27&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkMediaToProject'</v>
       </c>
       <c r="E29" t="str">
-        <f>IF('Restore Tree'!F44&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F44&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I29" t="str">
-        <f>IF('Restore Tree'!J56&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J56&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F31&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F31&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I29" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>IF('Restore Tree'!B43&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B43&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsFileSearchCandidates'</v>
+        <f>IF('Restore Tree'!B28&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B28&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Affiliates'</v>
       </c>
       <c r="E30" t="str">
-        <f>IF('Restore Tree'!F43&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F43&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F32&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F32&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I30" t="str">
-        <f>IF('Restore Tree'!J57&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J57&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J42&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J42&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>IF('Restore Tree'!B34&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B34&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkObjectToTask'</v>
+        <f>IF('Restore Tree'!B29&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B29&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectTargetCompaniesCandidates'</v>
       </c>
       <c r="E31" t="str">
-        <f>IF('Restore Tree'!F34&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F34&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F33&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F33&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I31" t="str">
-        <f>IF('Restore Tree'!J9&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J9&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J10&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J10&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>IF('Restore Tree'!B35&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B35&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B30&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B30&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsTargetLists'</v>
       </c>
       <c r="E32" t="str">
-        <f>IF('Restore Tree'!F35&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F35&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F34&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F34&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I32" t="str">
-        <f>IF('Restore Tree'!J58&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J58&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J52&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J52&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>IF('Restore Tree'!B56&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B56&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B31&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B31&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsSources'</v>
       </c>
       <c r="E33" t="str">
-        <f>IF('Restore Tree'!F56&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F56&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F35&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F35&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I33" t="str">
-        <f>IF('Restore Tree'!J10&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J10&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J11&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J11&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>IF('Restore Tree'!B57&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B57&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsCandidateBlocks'</v>
+        <f>IF('Restore Tree'!B32&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B32&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsFileSearchCandidates'</v>
       </c>
       <c r="E34" t="str">
-        <f>IF('Restore Tree'!F57&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F57&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I34" t="str">
-        <f>IF('Restore Tree'!J59&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J59&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F36&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F36&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I34" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>IF('Restore Tree'!B9&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B9&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectBillingDetails'</v>
+        <f>IF('Restore Tree'!B33&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B33&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsPresentedLists'</v>
       </c>
       <c r="E35" t="str">
-        <f>IF('Restore Tree'!F9&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F9&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F37&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F37&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'InternalInterviews'</v>
       </c>
       <c r="I35" t="str">
-        <f>IF('Restore Tree'!J11&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J11&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J12&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J12&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>IF('Restore Tree'!B27&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B27&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B34&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B34&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsBenchmarkCandidates'</v>
       </c>
       <c r="E36" t="str">
-        <f>IF('Restore Tree'!F27&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F27&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'SkillsQuestions'</v>
+        <f>IF('Restore Tree'!F38&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F38&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Interview'</v>
       </c>
       <c r="I36" t="str">
-        <f>IF('Restore Tree'!J12&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J12&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J13&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J13&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>IF('Restore Tree'!B28&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B28&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B35&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B35&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'PeopleAppliedTo'</v>
       </c>
       <c r="E37" t="str">
-        <f>IF('Restore Tree'!F28&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F28&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkWebPostingToWebSite'</v>
+        <f>IF('Restore Tree'!F39&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F39&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'CandidateCredentials'</v>
       </c>
       <c r="I37" t="str">
-        <f>IF('Restore Tree'!J54&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J54&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J50&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J50&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>IF('Restore Tree'!B29&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B29&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B36&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B36&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsClientEmployeesLists'</v>
       </c>
       <c r="E38" t="str">
-        <f>IF('Restore Tree'!F29&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F29&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I38" t="str">
-        <f>IF('Restore Tree'!J60&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J60&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F40&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F40&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'CandidateReferences'</v>
+      </c>
+      <c r="I38" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>IF('Restore Tree'!B58&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B58&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'People'</v>
+        <f>IF('Restore Tree'!B37&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B37&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsInternalInterviewLists'</v>
       </c>
       <c r="E39" t="str">
-        <f>IF('Restore Tree'!F58&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F58&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I39" t="str">
-        <f>IF('Restore Tree'!J61&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J61&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F41&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F41&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I39" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>IF('Restore Tree'!B10&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B10&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsAccounting'</v>
+        <f>IF('Restore Tree'!B38&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B38&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsShortLists'</v>
       </c>
       <c r="E40" t="str">
-        <f>IF('Restore Tree'!F10&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F10&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I40" t="str">
-        <f>IF('Restore Tree'!J62&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J62&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F42&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F42&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I40" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>IF('Restore Tree'!B59&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B59&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B39&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B39&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E41" t="str">
-        <f>IF('Restore Tree'!F59&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F59&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F43&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F43&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I41" t="str">
-        <f>IF('Restore Tree'!J13&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J13&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J14&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J14&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>IF('Restore Tree'!B11&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B11&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsClientTeams'</v>
+        <f>IF('Restore Tree'!B40&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B40&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E42" t="str">
-        <f>IF('Restore Tree'!F11&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F11&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkInterviewersToClientInterview'</v>
-      </c>
-      <c r="I42" t="str">
-        <f>IF('Restore Tree'!J63&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J63&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F44&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F44&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I42" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>IF('Restore Tree'!B12&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B12&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsCompaniesLists'</v>
+        <f>IF('Restore Tree'!B41&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B41&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'CandidateReferrals'</v>
       </c>
       <c r="E43" t="str">
-        <f>IF('Restore Tree'!F12&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F12&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectTargetCompaniesCandidates'</v>
-      </c>
-      <c r="I43" t="str">
-        <f>IF('Restore Tree'!J64&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J64&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F45&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F45&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I43" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>IF('Restore Tree'!B54&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B54&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Task'</v>
+        <f>IF('Restore Tree'!B42&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B42&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ProjectsCandidateBlocks'</v>
       </c>
       <c r="E44" t="str">
-        <f>IF('Restore Tree'!F54&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F54&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I44" t="str">
-        <f>IF('Restore Tree'!J65&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J65&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F46&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F46&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I44" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>IF('Restore Tree'!B60&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B60&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B43&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B43&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E45" t="str">
-        <f>IF('Restore Tree'!F60&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F60&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F47&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F47&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I45" t="str">
-        <f>IF('Restore Tree'!J14&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J14&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J15&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J15&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>IF('Restore Tree'!B61&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B61&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B44&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B44&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'ListsDetails'</v>
       </c>
       <c r="E46" t="str">
-        <f>IF('Restore Tree'!F61&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F61&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I46" t="str">
-        <f>IF('Restore Tree'!J66&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J66&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F48&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F48&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I46" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>IF('Restore Tree'!B62&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B62&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B45&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B45&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E47" t="str">
-        <f>IF('Restore Tree'!F62&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F62&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F49&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F49&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I47" t="str">
-        <f>IF('Restore Tree'!J37&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J37&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J27&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J27&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>IF('Restore Tree'!B13&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B13&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectsTeam'</v>
+        <f>IF('Restore Tree'!B46&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B46&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkObjectToActivityHistory'</v>
       </c>
       <c r="E48" t="str">
-        <f>IF('Restore Tree'!F13&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F13&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F50&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F50&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I48" t="str">
-        <f>IF('Restore Tree'!J15&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J15&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J16&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J16&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>IF('Restore Tree'!B36&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B36&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkEventsToBusinessObjects'</v>
+        <f>IF('Restore Tree'!B47&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B47&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkObjectToDocument'</v>
       </c>
       <c r="E49" t="str">
-        <f>IF('Restore Tree'!F36&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F36&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I49" t="str">
-        <f>IF('Restore Tree'!J68&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J68&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F51&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F51&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I49" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>IF('Restore Tree'!B63&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B63&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B48&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B48&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'LinkObjectToTask'</v>
       </c>
       <c r="E50" t="str">
-        <f>IF('Restore Tree'!F63&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F63&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F52&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F52&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I50" t="str">
-        <f>IF('Restore Tree'!J71&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J71&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J45&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J45&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>IF('Restore Tree'!B64&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B64&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B49&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B49&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E51" t="str">
-        <f>IF('Restore Tree'!F64&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F64&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F53&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F53&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I51" t="str">
-        <f>IF('Restore Tree'!J72&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J72&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J46&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J46&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>IF('Restore Tree'!B65&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B65&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B50&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B50&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Task'</v>
       </c>
       <c r="E52" t="str">
-        <f>IF('Restore Tree'!F65&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F65&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I52" t="str">
-        <f>IF('Restore Tree'!J73&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J73&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F54&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F54&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I52" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>IF('Restore Tree'!B14&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B14&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectStages'</v>
+        <f>IF('Restore Tree'!B51&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B51&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'WebRequests'</v>
       </c>
       <c r="E53" t="str">
-        <f>IF('Restore Tree'!F14&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F14&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkTaskToProjectStages'</v>
-      </c>
-      <c r="I53" t="str">
-        <f>IF('Restore Tree'!J74&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J74&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F55&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F55&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I53" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>IF('Restore Tree'!B66&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B66&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B52&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B52&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'People'</v>
       </c>
       <c r="E54" t="str">
-        <f>IF('Restore Tree'!F66&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F66&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I54" t="str">
-        <f>IF('Restore Tree'!J75&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J75&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F56&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F56&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I54" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>IF('Restore Tree'!B37&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B37&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkMediaToProject'</v>
+        <f>IF('Restore Tree'!B53&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B53&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E55" t="str">
-        <f>IF('Restore Tree'!F37&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F37&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I55" t="str">
-        <f>IF('Restore Tree'!J76&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J76&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F57&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F57&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I55" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>IF('Restore Tree'!B15&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B15&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ProjectInvoices'</v>
+        <f>IF('Restore Tree'!B54&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B54&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E56" t="str">
-        <f>IF('Restore Tree'!F15&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F15&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'InvoiceItems'</v>
-      </c>
-      <c r="I56" t="str">
-        <f>IF('Restore Tree'!J77&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J77&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F58&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F58&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I56" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>IF('Restore Tree'!B30&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B30&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ListsDetails'</v>
+        <f>IF('Restore Tree'!B55&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B55&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E57" t="str">
-        <f>IF('Restore Tree'!F30&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F30&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I57" t="str">
-        <f>IF('Restore Tree'!J78&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J78&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F59&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F59&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I57" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>IF('Restore Tree'!B31&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B31&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B56&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B56&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E58" t="str">
-        <f>IF('Restore Tree'!F31&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F31&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F60&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F60&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I58" t="str">
-        <f>IF('Restore Tree'!J79&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J79&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J49&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J49&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>IF('Restore Tree'!B32&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B32&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkObjectToActivityHistory'</v>
+        <f>IF('Restore Tree'!B57&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B57&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E59" t="str">
-        <f>IF('Restore Tree'!F32&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F32&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F61&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F61&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I59" t="str">
-        <f>IF('Restore Tree'!J16&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J16&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'DeletedTasks'</v>
+        <f>IF('Restore Tree'!J17&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J17&amp;"'", "")</f>
+        <v/>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>IF('Restore Tree'!B68&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B68&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B58&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B58&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E60" t="str">
-        <f>IF('Restore Tree'!F68&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F68&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I60" t="str">
-        <f>IF('Restore Tree'!J17&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J17&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'TaskData'</v>
+        <f>IF('Restore Tree'!F62&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F62&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I60" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>IF('Restore Tree'!B71&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B71&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B59&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B59&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E61" t="str">
-        <f>IF('Restore Tree'!F71&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F71&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I61" t="str">
-        <f>IF('Restore Tree'!J18&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J18&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkContactsToTask'</v>
+        <f>IF('Restore Tree'!F63&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F63&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I61" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f>IF('Restore Tree'!B72&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B72&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B60&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B60&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E62" t="str">
-        <f>IF('Restore Tree'!F72&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F72&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I62" t="str">
-        <f>IF('Restore Tree'!J19&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J19&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkTaskToProjectStages'</v>
+        <f>IF('Restore Tree'!F64&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F64&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I62" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>IF('Restore Tree'!B73&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B73&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B61&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B61&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E63" t="str">
-        <f>IF('Restore Tree'!F73&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F73&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I63" t="str">
-        <f>IF('Restore Tree'!J20&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J20&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkObjectToTask'</v>
+        <f>IF('Restore Tree'!F65&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F65&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I63" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>IF('Restore Tree'!B74&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B74&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B62&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B62&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Not Coded'</v>
       </c>
       <c r="E64" t="str">
-        <f>IF('Restore Tree'!F74&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F74&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F66&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F66&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I64" t="str">
-        <f>IF('Restore Tree'!J21&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J21&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J18&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J18&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f>IF('Restore Tree'!B75&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B75&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B63&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B63&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Not going to Code'</v>
       </c>
       <c r="E65" t="str">
-        <f>IF('Restore Tree'!F75&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F75&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F67&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F67&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I65" t="str">
-        <f>IF('Restore Tree'!J22&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J22&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J19&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J19&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f>IF('Restore Tree'!B76&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B76&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B64&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B64&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Coded'</v>
       </c>
       <c r="E66" t="str">
-        <f>IF('Restore Tree'!F76&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F76&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F68&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F68&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I66" t="str">
-        <f>IF('Restore Tree'!J23&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J23&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J20&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J20&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f>IF('Restore Tree'!B77&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B77&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B65&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B65&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Tested'</v>
       </c>
       <c r="E67" t="str">
-        <f>IF('Restore Tree'!F77&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F77&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F69&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F69&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I67" t="str">
-        <f>IF('Restore Tree'!J24&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J24&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J21&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J21&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f>IF('Restore Tree'!B78&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B78&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!B66&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B66&amp;"'", "")</f>
+        <v>exec sp_Drew_Restore_TableInfo @TableName = 'Not going to Test'</v>
       </c>
       <c r="E68" t="str">
-        <f>IF('Restore Tree'!F78&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F78&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I68" t="str">
-        <f>IF('Restore Tree'!J67&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J67&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F70&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F70&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I68" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>IF('Restore Tree'!B79&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B79&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B67&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B67&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E69" t="str">
-        <f>IF('Restore Tree'!F79&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F79&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F71&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F71&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I69" t="e">
@@ -4255,96 +4762,96 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>IF('Restore Tree'!B16&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B16&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'InternalInterviews'</v>
+        <f>IF('Restore Tree'!B68&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B68&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E70" t="str">
-        <f>IF('Restore Tree'!F16&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F16&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Task'</v>
-      </c>
-      <c r="I70" t="str">
-        <f>IF('Restore Tree'!J25&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J25&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F72&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F72&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I70" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f>IF('Restore Tree'!B17&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B17&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B69&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B69&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E71" t="str">
-        <f>IF('Restore Tree'!F17&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F17&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F73&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F73&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I71" t="str">
-        <f>IF('Restore Tree'!J26&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J26&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J22&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J22&amp;"'", "")</f>
         <v>exec sp_Drew_TableInfo @TableName = 'MultipleAnswerItems'</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f>IF('Restore Tree'!B18&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B18&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B70&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B70&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E72" t="str">
-        <f>IF('Restore Tree'!F18&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F18&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F74&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F74&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I72" t="str">
-        <f>IF('Restore Tree'!J27&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J27&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J23&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J23&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>IF('Restore Tree'!B19&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B19&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B71&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B71&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E73" t="str">
-        <f>IF('Restore Tree'!F19&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F19&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F75&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F75&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I73" t="str">
-        <f>IF('Restore Tree'!J28&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J28&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J24&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J24&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f>IF('Restore Tree'!B20&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B20&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B72&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B72&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E74" t="str">
-        <f>IF('Restore Tree'!F20&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F20&amp;"'", "")</f>
-        <v/>
-      </c>
-      <c r="I74" t="str">
-        <f>IF('Restore Tree'!J29&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J29&amp;"'", "")</f>
-        <v/>
+        <f>IF('Restore Tree'!F76&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F76&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I74" t="e">
+        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f>IF('Restore Tree'!B21&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B21&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B73&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B73&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E75" t="str">
-        <f>IF('Restore Tree'!F21&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F21&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkInternalInterviewsToResults'</v>
+        <f>IF('Restore Tree'!F77&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F77&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I75" t="str">
-        <f>IF('Restore Tree'!J36&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J36&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J26&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J26&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f>IF('Restore Tree'!B22&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B22&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B74&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B74&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E76" t="str">
-        <f>IF('Restore Tree'!F22&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F22&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkSkillsToInternalInterview'</v>
+        <f>IF('Restore Tree'!F78&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F78&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I76" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4353,12 +4860,12 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f>IF('Restore Tree'!B23&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B23&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Interview'</v>
+        <f>IF('Restore Tree'!B75&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B75&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E77" t="str">
-        <f>IF('Restore Tree'!F23&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F23&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Task'</v>
+        <f>IF('Restore Tree'!F79&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F79&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I77" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4367,12 +4874,12 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f>IF('Restore Tree'!B24&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B24&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B76&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B76&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E78" t="str">
-        <f>IF('Restore Tree'!F24&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F24&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkInterviewersToClientInterview'</v>
+        <f>IF('Restore Tree'!F80&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F80&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I78" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4381,54 +4888,54 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f>IF('Restore Tree'!B67&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B67&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B77&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B77&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E79" t="str">
-        <f>IF('Restore Tree'!F67&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F67&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F81&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F81&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I79" t="str">
-        <f>IF('Restore Tree'!J30&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J30&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J44&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J44&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" t="e">
+      <c r="A80" t="str">
+        <f>IF('Restore Tree'!B78&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B78&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E80" t="str">
+        <f>IF('Restore Tree'!F82&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F82&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="I80" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
         <v>#REF!</v>
       </c>
-      <c r="E80" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I80" t="str">
-        <f>IF('Restore Tree'!J31&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J31&amp;"'", "")</f>
-        <v/>
-      </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f>IF('Restore Tree'!B25&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B25&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B79&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B79&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E81" t="str">
-        <f>IF('Restore Tree'!F25&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F25&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkClnInterviewsToResults'</v>
+        <f>IF('Restore Tree'!F83&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F83&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I81" t="str">
-        <f>IF('Restore Tree'!J32&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J32&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J47&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J47&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
-        <f>IF('Restore Tree'!B26&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B26&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'WebJobPostings'</v>
+        <f>IF('Restore Tree'!B80&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B80&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E82" t="str">
-        <f>IF('Restore Tree'!F26&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F26&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'Questions'</v>
+        <f>IF('Restore Tree'!F84&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F84&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I82" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4437,12 +4944,12 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f>IF('Restore Tree'!B27&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B27&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B81&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B81&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E83" t="str">
-        <f>IF('Restore Tree'!F27&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F27&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'SkillsQuestions'</v>
+        <f>IF('Restore Tree'!F85&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F85&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I83" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4451,12 +4958,12 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
-        <f>IF('Restore Tree'!B28&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B28&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B82&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B82&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E84" t="str">
-        <f>IF('Restore Tree'!F28&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F28&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkWebPostingToWebSite'</v>
+        <f>IF('Restore Tree'!F86&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F86&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I84" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4465,11 +4972,11 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f>IF('Restore Tree'!B29&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B29&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B83&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B83&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E85" t="str">
-        <f>IF('Restore Tree'!F29&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F29&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F87&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F87&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I85" t="e">
@@ -4479,11 +4986,11 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f>IF('Restore Tree'!B36&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B36&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkEventsToBusinessObjects'</v>
+        <f>IF('Restore Tree'!B84&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B84&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E86" t="str">
-        <f>IF('Restore Tree'!F36&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F36&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F88&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F88&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I86" t="e">
@@ -4493,11 +5000,11 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f>IF('Restore Tree'!B64&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B64&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B85&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B85&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E87" t="str">
-        <f>IF('Restore Tree'!F64&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F64&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F89&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F89&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I87" t="e">
@@ -4507,11 +5014,11 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f>IF('Restore Tree'!B30&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B30&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'ListsDetails'</v>
+        <f>IF('Restore Tree'!B86&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B86&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E88" t="str">
-        <f>IF('Restore Tree'!F30&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F30&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F90&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F90&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I88" t="e">
@@ -4521,11 +5028,11 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>IF('Restore Tree'!B31&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B31&amp;"'", "")</f>
+        <f>IF('Restore Tree'!B87&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B87&amp;"'", "")</f>
         <v/>
       </c>
       <c r="E89" t="str">
-        <f>IF('Restore Tree'!F31&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F31&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F91&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F91&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I89" t="e">
@@ -4535,11 +5042,11 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
-        <f>IF('Restore Tree'!B32&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!B32&amp;"'", "")</f>
-        <v>exec sp_Drew_TableInfo @TableName = 'LinkObjectToActivityHistory'</v>
+        <f>IF('Restore Tree'!B88&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B88&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="E90" t="str">
-        <f>IF('Restore Tree'!F32&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!F32&amp;"'", "")</f>
+        <f>IF('Restore Tree'!F92&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F92&amp;"'", "")</f>
         <v/>
       </c>
       <c r="I90" t="e">
@@ -4548,13 +5055,13 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E91" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+      <c r="A91" t="str">
+        <f>IF('Restore Tree'!B89&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B89&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E91" t="str">
+        <f>IF('Restore Tree'!F93&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F93&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I91" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4562,13 +5069,13 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E92" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+      <c r="A92" t="str">
+        <f>IF('Restore Tree'!B90&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B90&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E92" t="str">
+        <f>IF('Restore Tree'!F94&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F94&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I92" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4576,13 +5083,13 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E93" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+      <c r="A93" t="str">
+        <f>IF('Restore Tree'!B91&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B91&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E93" t="str">
+        <f>IF('Restore Tree'!F95&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F95&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I93" t="e">
         <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
@@ -4590,132 +5097,192 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E94" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+      <c r="A94" t="str">
+        <f>IF('Restore Tree'!B92&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B92&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E94" t="str">
+        <f>IF('Restore Tree'!F96&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F96&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I94" t="str">
-        <f>IF('Restore Tree'!J80&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J80&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J53&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J53&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E95" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+      <c r="A95" t="str">
+        <f>IF('Restore Tree'!B93&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B93&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E95" t="str">
+        <f>IF('Restore Tree'!F97&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F97&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I95" t="str">
-        <f>IF('Restore Tree'!J81&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J81&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J54&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J54&amp;"'", "")</f>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E96" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+      <c r="A96" t="str">
+        <f>IF('Restore Tree'!B94&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B94&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E96" t="str">
+        <f>IF('Restore Tree'!F98&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F98&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I96" t="str">
-        <f>IF('Restore Tree'!J82&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J82&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E97" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+        <f>IF('Restore Tree'!J55&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J55&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f>IF('Restore Tree'!B95&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B95&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E97" t="str">
+        <f>IF('Restore Tree'!F99&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F99&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I97" t="str">
-        <f>IF('Restore Tree'!J83&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J83&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E98" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+        <f>IF('Restore Tree'!J56&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J56&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f>IF('Restore Tree'!B96&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B96&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E98" t="str">
+        <f>IF('Restore Tree'!F100&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F100&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I98" t="str">
-        <f>IF('Restore Tree'!J84&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J84&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E99" t="e">
-        <f>IF('Restore Tree'!#REF!&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!#REF!&amp;"'", "")</f>
-        <v>#REF!</v>
+        <f>IF('Restore Tree'!J57&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J57&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f>IF('Restore Tree'!B97&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B97&amp;"'", "")</f>
+        <v/>
+      </c>
+      <c r="E99" t="str">
+        <f>IF('Restore Tree'!F101&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!F101&amp;"'", "")</f>
+        <v/>
       </c>
       <c r="I99" t="str">
-        <f>IF('Restore Tree'!J85&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J85&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J58&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J58&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f>IF('Restore Tree'!B98&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B98&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I100" t="str">
-        <f>IF('Restore Tree'!J86&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J86&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J59&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J59&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
+        <f>IF('Restore Tree'!B99&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B99&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I101" t="str">
-        <f>IF('Restore Tree'!J87&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J87&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="102" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J60&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J60&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f>IF('Restore Tree'!B100&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B100&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I102" t="str">
-        <f>IF('Restore Tree'!J88&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J88&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="103" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J61&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J61&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="str">
+        <f>IF('Restore Tree'!B101&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B101&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I103" t="str">
-        <f>IF('Restore Tree'!J89&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J89&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="104" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J62&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J62&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="str">
+        <f>IF('Restore Tree'!B102&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B102&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I104" t="str">
-        <f>IF('Restore Tree'!J91&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J91&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="105" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J64&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J64&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="str">
+        <f>IF('Restore Tree'!B103&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B103&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I105" t="str">
-        <f>IF('Restore Tree'!J92&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J92&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J65&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J65&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" t="str">
+        <f>IF('Restore Tree'!B104&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B104&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I106" t="str">
-        <f>IF('Restore Tree'!J93&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J93&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="107" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J66&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J66&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="str">
+        <f>IF('Restore Tree'!B105&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B105&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I107" t="str">
-        <f>IF('Restore Tree'!J94&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J94&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="108" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J67&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J67&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="str">
+        <f>IF('Restore Tree'!B106&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B106&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I108" t="str">
-        <f>IF('Restore Tree'!J95&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J95&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="109" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J68&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J68&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="str">
+        <f>IF('Restore Tree'!B107&gt;"","exec sp_Drew_Restore_TableInfo @TableName = '"&amp;'Restore Tree'!B107&amp;"'", "")</f>
+        <v/>
+      </c>
       <c r="I109" t="str">
-        <f>IF('Restore Tree'!J96&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J96&amp;"'", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="5:9" x14ac:dyDescent="0.25">
+        <f>IF('Restore Tree'!J69&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J69&amp;"'", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I110" t="str">
-        <f>IF('Restore Tree'!J97&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J97&amp;"'", "")</f>
+        <f>IF('Restore Tree'!J70&gt;"","exec sp_Drew_TableInfo @TableName = '"&amp;'Restore Tree'!J70&amp;"'", "")</f>
         <v/>
       </c>
     </row>
@@ -4724,7 +5291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E47788-62EB-482C-B79D-4D43E2B072DF}">
   <dimension ref="A1:D63"/>
   <sheetViews>
@@ -4740,7 +5307,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="5" t="str">
@@ -4751,7 +5318,7 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="str">
@@ -4762,7 +5329,7 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="5" t="str">
@@ -4773,7 +5340,7 @@
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="5" t="str">
@@ -4784,7 +5351,7 @@
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="5" t="str">
@@ -4795,7 +5362,7 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="5" t="str">
@@ -4806,7 +5373,7 @@
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B7" s="5" t="str">
@@ -4817,7 +5384,7 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="5" t="str">
@@ -4828,7 +5395,7 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5" t="str">
@@ -4839,7 +5406,7 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="5" t="str">
@@ -4850,7 +5417,7 @@
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B11" s="5" t="str">
@@ -4861,7 +5428,7 @@
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="5" t="str">
@@ -4872,7 +5439,7 @@
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="5" t="str">
@@ -4883,7 +5450,7 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="5" t="str">
@@ -4894,7 +5461,7 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="5" t="str">
@@ -4905,7 +5472,7 @@
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="5" t="str">
@@ -4916,7 +5483,7 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="15" t="s">
         <v>95</v>
       </c>
       <c r="B17" s="5" t="str">
@@ -4927,7 +5494,7 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="5" t="str">
@@ -4940,7 +5507,7 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="5" t="str">
@@ -4953,7 +5520,7 @@
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="5" t="str">
@@ -4966,7 +5533,7 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="5" t="str">
@@ -4979,7 +5546,7 @@
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="5" t="str">
@@ -4990,7 +5557,7 @@
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="5" t="str">
@@ -5003,7 +5570,7 @@
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="5" t="str">
@@ -5014,7 +5581,7 @@
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="5" t="str">
@@ -5025,7 +5592,7 @@
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="5" t="str">
@@ -5036,7 +5603,7 @@
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="5" t="str">
@@ -5047,7 +5614,7 @@
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="5" t="str">
@@ -5058,7 +5625,7 @@
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="5" t="str">
@@ -5069,7 +5636,7 @@
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="5" t="str">
@@ -5080,7 +5647,7 @@
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="5" t="str">
@@ -5091,7 +5658,7 @@
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="5" t="str">
@@ -5102,7 +5669,7 @@
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="5" t="str">
@@ -5113,7 +5680,7 @@
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="5" t="str">
@@ -5124,7 +5691,7 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="5" t="str">
@@ -5135,7 +5702,7 @@
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="5" t="str">
@@ -5146,7 +5713,7 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B37" s="5" t="str">
@@ -5157,7 +5724,7 @@
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="5" t="str">
@@ -5168,7 +5735,7 @@
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="5" t="str">
@@ -5179,7 +5746,7 @@
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B40" s="5" t="str">
@@ -5190,7 +5757,7 @@
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="5" t="str">
@@ -5201,7 +5768,7 @@
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="15" t="s">
         <v>59</v>
       </c>
       <c r="B42" s="5" t="str">
@@ -5212,7 +5779,7 @@
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B43" s="5" t="str">
@@ -5223,7 +5790,7 @@
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B44" s="5" t="str">
@@ -5234,7 +5801,7 @@
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B45" s="5" t="str">
@@ -5245,7 +5812,7 @@
       <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B46" s="5" t="str">
@@ -5256,7 +5823,7 @@
       <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="5" t="str">
@@ -5267,7 +5834,7 @@
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B48" s="5" t="str">
@@ -5278,7 +5845,7 @@
       <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B49" s="5" t="str">
@@ -5289,7 +5856,7 @@
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="5" t="str">
@@ -5300,7 +5867,7 @@
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B51" s="5" t="str">
@@ -5315,7 +5882,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B52" s="5" t="str">
@@ -5326,7 +5893,7 @@
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B53" s="5" t="str">
@@ -5341,52 +5908,52 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="5" t="str">
         <f t="shared" si="0"/>
         <v>('LinkObjectToActivityHistory', N'WHERE PeopleID = @MainRecordID'),</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B55" s="5" t="str">
         <f t="shared" si="0"/>
         <v>('LinkObjectToDocument', N'WHERE PeopleID = @MainRecordID'),</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B56" s="5" t="str">
         <f t="shared" si="0"/>
         <v>('LinkObjectToTask', N'WHERE PeopleID = @MainRecordID'),</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="16" t="s">
         <v>76</v>
       </c>
       <c r="B57" s="5" t="str">
@@ -5399,7 +5966,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="17" t="s">
         <v>76</v>
       </c>
       <c r="B58" s="5" t="str">
@@ -5412,7 +5979,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B59" s="5" t="str">
@@ -5425,7 +5992,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="5" t="str">
@@ -5433,12 +6000,12 @@
         <v>('JobOrders', N'WHERE PeopleID = @MainRecordID'),</v>
       </c>
       <c r="C60" s="11"/>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B61" s="5" t="str">
@@ -5446,12 +6013,12 @@
         <v>('JobOrders', N'WHERE PeopleID = @MainRecordID'),</v>
       </c>
       <c r="C61" s="11"/>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B62" s="5" t="str">
@@ -5459,12 +6026,12 @@
         <v>('JobOrders', N'WHERE PeopleID = @MainRecordID'),</v>
       </c>
       <c r="C62" s="11"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="18" t="s">
         <v>78</v>
       </c>
       <c r="B63" s="5" t="str">
@@ -5481,7 +6048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CAA956-DEDF-4BA1-9030-19D401808C4D}">
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -5496,10 +6063,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>85</v>
       </c>
       <c r="C1" s="5"/>
@@ -5511,10 +6078,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -5528,10 +6095,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="15" t="s">
         <v>87</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -5545,10 +6112,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="15" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -5562,10 +6129,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="15" t="s">
         <v>89</v>
       </c>
       <c r="C5" s="5"/>
@@ -5577,10 +6144,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="15" t="s">
         <v>90</v>
       </c>
       <c r="C6" s="5"/>
@@ -5592,10 +6159,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="15" t="s">
         <v>91</v>
       </c>
       <c r="C7" s="5"/>
@@ -5607,10 +6174,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5"/>
@@ -5624,10 +6191,10 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>97</v>
       </c>
       <c r="K9" t="str">
@@ -5636,10 +6203,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="15" t="s">
         <v>96</v>
       </c>
       <c r="K10" t="str">
@@ -5648,10 +6215,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>94</v>
       </c>
       <c r="K11" t="str">
@@ -5660,10 +6227,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>100</v>
       </c>
       <c r="K12" t="str">
@@ -5672,10 +6239,10 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="15" t="s">
         <v>0</v>
       </c>
       <c r="K13" t="str">
@@ -5684,10 +6251,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="15" t="s">
         <v>6</v>
       </c>
       <c r="K14" t="str">
@@ -5696,10 +6263,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="15" t="s">
         <v>98</v>
       </c>
       <c r="K15" t="str">
@@ -5708,10 +6275,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="15" t="s">
         <v>99</v>
       </c>
       <c r="K16" t="str">
@@ -5720,10 +6287,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="5"/>

</xml_diff>